<commit_message>
modif stat dpt  pb => % et undefined
</commit_message>
<xml_diff>
--- a/export_equipeDPT.xlsx
+++ b/export_equipeDPT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothée\Desktop\temp\export_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothée\Desktop\EXCEL\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822C69A6-4B52-4465-858B-3FEEE7F10697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6506F0ED-CEDF-4D9C-8FFB-84CEECED0D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="1545" windowWidth="25515" windowHeight="21585" xr2:uid="{F6DAA3BA-2FBE-49B1-8799-244C6D03BB2F}"/>
+    <workbookView xWindow="2205" yWindow="1125" windowWidth="33675" windowHeight="21585" xr2:uid="{F6DAA3BA-2FBE-49B1-8799-244C6D03BB2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>Secteur</t>
   </si>
@@ -172,6 +172,9 @@
       </rPr>
       <t xml:space="preserve"> rattachées au seteur CD08</t>
     </r>
+  </si>
+  <si>
+    <t>31!</t>
   </si>
 </sst>
 </file>
@@ -876,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97309776-FEF6-4B26-A2B7-99861F3976E5}">
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,8 +1764,8 @@
       <c r="A46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="77">
-        <v>31</v>
+      <c r="B46" s="77" t="s">
+        <v>38</v>
       </c>
       <c r="C46" s="37">
         <v>4</v>

</xml_diff>